<commit_message>
Commit changes before 12 oclock
</commit_message>
<xml_diff>
--- a/Scrum/Backlogs/Backlog Week 4.xlsx
+++ b/Scrum/Backlogs/Backlog Week 4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\template\Scrum\Retrospective\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\template\Scrum\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06AE72E-8267-4EBF-ADD5-BE1513E14B71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110E274E-0DDB-4A1C-B311-A9B4E0534FE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,9 +76,6 @@
     <t>Johannes</t>
   </si>
   <si>
-    <t>Week 3</t>
-  </si>
-  <si>
     <t>I am a developer and I need a place to store my users data</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>4 each</t>
+  </si>
+  <si>
+    <t>Week 4</t>
   </si>
 </sst>
 </file>
@@ -646,8 +646,8 @@
   </sheetPr>
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
@@ -962,7 +962,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
@@ -1059,16 +1059,16 @@
     <row r="14" spans="1:26" ht="52.8">
       <c r="A14" s="1"/>
       <c r="B14" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" s="26">
         <v>4</v>
@@ -1099,16 +1099,16 @@
     <row r="15" spans="1:26" ht="39.6">
       <c r="A15" s="1"/>
       <c r="B15" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="26">
         <v>4</v>
@@ -1142,13 +1142,13 @@
         <v>15</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="26">
         <v>4</v>
@@ -1179,22 +1179,22 @@
     <row r="17" spans="1:26" ht="52.8">
       <c r="A17" s="1"/>
       <c r="B17" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="26">
         <v>4</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1219,22 +1219,22 @@
     <row r="18" spans="1:26" ht="26.4">
       <c r="A18" s="1"/>
       <c r="B18" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" s="26">
         <v>4</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1259,16 +1259,16 @@
     <row r="19" spans="1:26" ht="39.6">
       <c r="A19" s="1"/>
       <c r="B19" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="26">
         <v>4</v>

</xml_diff>